<commit_message>
OBJ Model Loadig Prototype ( Partially complete )
Some of the sides aren't rendering properly, maybe I need to modify my indexer for those sides specifically.
</commit_message>
<xml_diff>
--- a/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
+++ b/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2300" yWindow="700" windowWidth="30380" windowHeight="17280"/>
+    <workbookView xWindow="3620" yWindow="1580" windowWidth="30380" windowHeight="17280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
@@ -1095,7 +1095,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:12">
@@ -1111,11 +1111,15 @@
       <c r="D5" s="5">
         <v>2</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3"/>
+      <c r="E5" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G5" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H5" s="5" t="s">
         <v>27</v>
@@ -1224,7 +1228,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1479,7 +1483,9 @@
       <c r="D19" s="5">
         <v>4</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="16">
         <f t="shared" si="0"/>
@@ -1504,7 +1510,9 @@
       <c r="D20" s="5">
         <v>3</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="16">
         <f t="shared" si="0"/>
@@ -2473,7 +2481,9 @@
       <c r="D63" s="5">
         <v>1</v>
       </c>
-      <c r="E63" s="2"/>
+      <c r="E63" s="2" t="s">
+        <v>95</v>
+      </c>
       <c r="F63" s="3"/>
       <c r="G63" s="16">
         <f t="shared" si="1"/>

</xml_diff>

<commit_message>
Render to Goemetry Done (but messy)
</commit_message>
<xml_diff>
--- a/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
+++ b/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
@@ -1,17 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="21405"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="3620" yWindow="1580" windowWidth="30380" windowHeight="17280"/>
+    <workbookView xWindow="4545" yWindow="1575" windowWidth="30375" windowHeight="17280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -26,7 +26,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0">
+    <comment ref="A2" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0">
+    <comment ref="A66" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="96">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -377,7 +377,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -951,26 +951,26 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="106.5" customWidth="1"/>
-    <col min="2" max="2" width="25.5" customWidth="1"/>
+    <col min="1" max="1" width="106.42578125" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" customWidth="1"/>
     <col min="3" max="3" width="25" customWidth="1"/>
-    <col min="4" max="4" width="25.33203125" customWidth="1"/>
-    <col min="5" max="6" width="25.5" customWidth="1"/>
-    <col min="7" max="7" width="25.6640625" customWidth="1"/>
-    <col min="8" max="9" width="25.83203125" customWidth="1"/>
-    <col min="10" max="10" width="24.6640625" customWidth="1"/>
-    <col min="11" max="11" width="24.5" customWidth="1"/>
-    <col min="12" max="12" width="24.1640625" customWidth="1"/>
-    <col min="13" max="14" width="9.1640625" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="6" width="25.42578125" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" customWidth="1"/>
+    <col min="8" max="9" width="25.85546875" customWidth="1"/>
+    <col min="10" max="10" width="24.7109375" customWidth="1"/>
+    <col min="11" max="11" width="24.42578125" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" customWidth="1"/>
+    <col min="13" max="14" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>92</v>
       </c>
@@ -986,7 +986,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" ht="15.75" customHeight="1">
+    <row r="2" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>93</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:12">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>63</v>
       </c>
@@ -1054,7 +1054,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:12">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
         <v>67</v>
       </c>
@@ -1083,7 +1083,7 @@
       </c>
       <c r="I4" s="17">
         <f>IF(SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=II",G4:G81) + SUMIF(D83:D84, "X",B83:B84))</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
@@ -1095,10 +1095,10 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>51</v>
       </c>
@@ -1135,7 +1135,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:12">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>34</v>
       </c>
@@ -1172,7 +1172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>52</v>
       </c>
@@ -1203,7 +1203,7 @@
       <c r="K7" s="5"/>
       <c r="L7" s="5"/>
     </row>
-    <row r="8" spans="1:12">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>35</v>
       </c>
@@ -1228,7 +1228,7 @@
       </c>
       <c r="I8" s="17">
         <f>I4+IF(I4 &lt; 18, IF(H10+I4 &gt; 18, 18- I4, H10),0)</f>
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
@@ -1237,7 +1237,7 @@
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
     </row>
-    <row r="9" spans="1:12">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>36</v>
       </c>
@@ -1268,7 +1268,7 @@
       <c r="K9" s="5"/>
       <c r="L9" s="5"/>
     </row>
-    <row r="10" spans="1:12">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>64</v>
       </c>
@@ -1302,7 +1302,7 @@
       <c r="K10" s="5"/>
       <c r="L10" s="5"/>
     </row>
-    <row r="11" spans="1:12">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>37</v>
       </c>
@@ -1327,7 +1327,7 @@
       <c r="K11" s="5"/>
       <c r="L11" s="5"/>
     </row>
-    <row r="12" spans="1:12">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="8"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -1344,7 +1344,7 @@
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
     </row>
-    <row r="13" spans="1:12">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>61</v>
       </c>
@@ -1363,7 +1363,7 @@
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
     </row>
-    <row r="14" spans="1:12">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="8"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -1380,7 +1380,7 @@
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
     </row>
-    <row r="15" spans="1:12">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="8"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1397,7 +1397,7 @@
       <c r="K15" s="5"/>
       <c r="L15" s="5"/>
     </row>
-    <row r="16" spans="1:12">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>10</v>
       </c>
@@ -1416,7 +1416,7 @@
       <c r="K16" s="5"/>
       <c r="L16" s="5"/>
     </row>
-    <row r="17" spans="1:12">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
         <v>39</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="K17" s="5"/>
       <c r="L17" s="5"/>
     </row>
-    <row r="18" spans="1:12">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>60</v>
       </c>
@@ -1470,7 +1470,7 @@
       <c r="K18" s="5"/>
       <c r="L18" s="5"/>
     </row>
-    <row r="19" spans="1:12">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
         <v>40</v>
       </c>
@@ -1486,10 +1486,12 @@
       <c r="E19" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="F19" s="3"/>
+      <c r="F19" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G19" s="16">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
@@ -1497,7 +1499,7 @@
       <c r="K19" s="5"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
         <v>38</v>
       </c>
@@ -1524,7 +1526,7 @@
       <c r="K20" s="5"/>
       <c r="L20" s="5"/>
     </row>
-    <row r="21" spans="1:12">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="20" t="s">
         <v>53</v>
       </c>
@@ -1549,7 +1551,7 @@
       <c r="K21" s="5"/>
       <c r="L21" s="5"/>
     </row>
-    <row r="22" spans="1:12">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="8"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -1566,7 +1568,7 @@
       <c r="K22" s="5"/>
       <c r="L22" s="5"/>
     </row>
-    <row r="23" spans="1:12">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="8"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -1583,7 +1585,7 @@
       <c r="K23" s="5"/>
       <c r="L23" s="5"/>
     </row>
-    <row r="24" spans="1:12">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="9" t="s">
         <v>9</v>
       </c>
@@ -1602,7 +1604,7 @@
       <c r="K24" s="5"/>
       <c r="L24" s="5"/>
     </row>
-    <row r="25" spans="1:12">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="10" t="s">
         <v>41</v>
       </c>
@@ -1627,7 +1629,7 @@
       <c r="K25" s="5"/>
       <c r="L25" s="5"/>
     </row>
-    <row r="26" spans="1:12">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="10" t="s">
         <v>42</v>
       </c>
@@ -1652,7 +1654,7 @@
       <c r="K26" s="5"/>
       <c r="L26" s="5"/>
     </row>
-    <row r="27" spans="1:12">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="10" t="s">
         <v>43</v>
       </c>
@@ -1677,7 +1679,7 @@
       <c r="K27" s="5"/>
       <c r="L27" s="5"/>
     </row>
-    <row r="28" spans="1:12">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>44</v>
       </c>
@@ -1702,7 +1704,7 @@
       <c r="K28" s="5"/>
       <c r="L28" s="5"/>
     </row>
-    <row r="29" spans="1:12">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>45</v>
       </c>
@@ -1727,7 +1729,7 @@
       <c r="K29" s="5"/>
       <c r="L29" s="5"/>
     </row>
-    <row r="30" spans="1:12">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>46</v>
       </c>
@@ -1752,7 +1754,7 @@
       <c r="K30" s="5"/>
       <c r="L30" s="5"/>
     </row>
-    <row r="31" spans="1:12">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>47</v>
       </c>
@@ -1777,7 +1779,7 @@
       <c r="K31" s="5"/>
       <c r="L31" s="5"/>
     </row>
-    <row r="32" spans="1:12">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>59</v>
       </c>
@@ -1802,7 +1804,7 @@
       <c r="K32" s="5"/>
       <c r="L32" s="5"/>
     </row>
-    <row r="33" spans="1:12">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>68</v>
       </c>
@@ -1827,7 +1829,7 @@
       <c r="K33" s="5"/>
       <c r="L33" s="5"/>
     </row>
-    <row r="34" spans="1:12">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>69</v>
       </c>
@@ -1852,7 +1854,7 @@
       <c r="K34" s="5"/>
       <c r="L34" s="5"/>
     </row>
-    <row r="35" spans="1:12">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>54</v>
       </c>
@@ -1877,7 +1879,7 @@
       <c r="K35" s="5"/>
       <c r="L35" s="5"/>
     </row>
-    <row r="36" spans="1:12">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="11"/>
       <c r="B36" s="5"/>
       <c r="C36" s="5"/>
@@ -1894,7 +1896,7 @@
       <c r="K36" s="5"/>
       <c r="L36" s="5"/>
     </row>
-    <row r="37" spans="1:12">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="11"/>
       <c r="B37" s="5"/>
       <c r="C37" s="5"/>
@@ -1911,7 +1913,7 @@
       <c r="K37" s="5"/>
       <c r="L37" s="5"/>
     </row>
-    <row r="38" spans="1:12">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>82</v>
       </c>
@@ -1930,7 +1932,7 @@
       <c r="K38" s="5"/>
       <c r="L38" s="5"/>
     </row>
-    <row r="39" spans="1:12">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>81</v>
       </c>
@@ -1955,7 +1957,7 @@
       <c r="K39" s="5"/>
       <c r="L39" s="5"/>
     </row>
-    <row r="40" spans="1:12">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>84</v>
       </c>
@@ -1980,7 +1982,7 @@
       <c r="K40" s="5"/>
       <c r="L40" s="5"/>
     </row>
-    <row r="41" spans="1:12">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>83</v>
       </c>
@@ -2005,7 +2007,7 @@
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
     </row>
-    <row r="42" spans="1:12">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>85</v>
       </c>
@@ -2030,7 +2032,7 @@
       <c r="K42" s="5"/>
       <c r="L42" s="5"/>
     </row>
-    <row r="43" spans="1:12">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>86</v>
       </c>
@@ -2055,7 +2057,7 @@
       <c r="K43" s="5"/>
       <c r="L43" s="5"/>
     </row>
-    <row r="44" spans="1:12">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44" s="8"/>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2072,7 +2074,7 @@
       <c r="K44" s="5"/>
       <c r="L44" s="5"/>
     </row>
-    <row r="45" spans="1:12">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45" s="8"/>
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
@@ -2089,7 +2091,7 @@
       <c r="K45" s="5"/>
       <c r="L45" s="5"/>
     </row>
-    <row r="46" spans="1:12">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="9" t="s">
         <v>8</v>
       </c>
@@ -2108,7 +2110,7 @@
       <c r="K46" s="5"/>
       <c r="L46" s="5"/>
     </row>
-    <row r="47" spans="1:12">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>58</v>
       </c>
@@ -2133,7 +2135,7 @@
       <c r="K47" s="5"/>
       <c r="L47" s="5"/>
     </row>
-    <row r="48" spans="1:12">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>55</v>
       </c>
@@ -2158,7 +2160,7 @@
       <c r="K48" s="5"/>
       <c r="L48" s="5"/>
     </row>
-    <row r="49" spans="1:12">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>65</v>
       </c>
@@ -2183,7 +2185,7 @@
       <c r="K49" s="5"/>
       <c r="L49" s="5"/>
     </row>
-    <row r="50" spans="1:12">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50" s="8"/>
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
@@ -2200,7 +2202,7 @@
       <c r="K50" s="5"/>
       <c r="L50" s="5"/>
     </row>
-    <row r="51" spans="1:12">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51" s="8"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -2217,7 +2219,7 @@
       <c r="K51" s="5"/>
       <c r="L51" s="5"/>
     </row>
-    <row r="52" spans="1:12">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
         <v>7</v>
       </c>
@@ -2236,7 +2238,7 @@
       <c r="K52" s="5"/>
       <c r="L52" s="5"/>
     </row>
-    <row r="53" spans="1:12">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>48</v>
       </c>
@@ -2261,7 +2263,7 @@
       <c r="K53" s="5"/>
       <c r="L53" s="5"/>
     </row>
-    <row r="54" spans="1:12">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54" s="11" t="s">
         <v>80</v>
       </c>
@@ -2286,7 +2288,7 @@
       <c r="K54" s="5"/>
       <c r="L54" s="5"/>
     </row>
-    <row r="55" spans="1:12">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55" s="11" t="s">
         <v>87</v>
       </c>
@@ -2311,7 +2313,7 @@
       <c r="K55" s="5"/>
       <c r="L55" s="5"/>
     </row>
-    <row r="56" spans="1:12">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56" s="11" t="s">
         <v>56</v>
       </c>
@@ -2336,7 +2338,7 @@
       <c r="K56" s="5"/>
       <c r="L56" s="5"/>
     </row>
-    <row r="57" spans="1:12">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="8"/>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
@@ -2353,7 +2355,7 @@
       <c r="K57" s="5"/>
       <c r="L57" s="5"/>
     </row>
-    <row r="58" spans="1:12">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58" s="8"/>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
@@ -2370,7 +2372,7 @@
       <c r="K58" s="5"/>
       <c r="L58" s="5"/>
     </row>
-    <row r="59" spans="1:12">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
         <v>6</v>
       </c>
@@ -2389,7 +2391,7 @@
       <c r="K59" s="5"/>
       <c r="L59" s="5"/>
     </row>
-    <row r="60" spans="1:12">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60" s="10" t="s">
         <v>88</v>
       </c>
@@ -2416,7 +2418,7 @@
       <c r="K60" s="5"/>
       <c r="L60" s="5"/>
     </row>
-    <row r="61" spans="1:12">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61" s="10" t="s">
         <v>89</v>
       </c>
@@ -2443,7 +2445,7 @@
       <c r="K61" s="5"/>
       <c r="L61" s="5"/>
     </row>
-    <row r="62" spans="1:12">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62" s="10" t="s">
         <v>70</v>
       </c>
@@ -2468,7 +2470,7 @@
       <c r="K62" s="5"/>
       <c r="L62" s="5"/>
     </row>
-    <row r="63" spans="1:12">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63" s="10" t="s">
         <v>71</v>
       </c>
@@ -2495,7 +2497,7 @@
       <c r="K63" s="5"/>
       <c r="L63" s="5"/>
     </row>
-    <row r="64" spans="1:12">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64" s="10" t="s">
         <v>72</v>
       </c>
@@ -2520,7 +2522,7 @@
       <c r="K64" s="5"/>
       <c r="L64" s="5"/>
     </row>
-    <row r="65" spans="1:12">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65" s="21" t="s">
         <v>66</v>
       </c>
@@ -2549,7 +2551,7 @@
       <c r="K65" s="5"/>
       <c r="L65" s="5"/>
     </row>
-    <row r="66" spans="1:12">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66" s="10" t="s">
         <v>57</v>
       </c>
@@ -2574,7 +2576,7 @@
       <c r="K66" s="5"/>
       <c r="L66" s="5"/>
     </row>
-    <row r="67" spans="1:12">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67" s="8"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -2591,7 +2593,7 @@
       <c r="K67" s="5"/>
       <c r="L67" s="5"/>
     </row>
-    <row r="68" spans="1:12">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
       <c r="B68" s="1"/>
       <c r="C68" s="1"/>
@@ -2608,7 +2610,7 @@
       <c r="K68" s="5"/>
       <c r="L68" s="5"/>
     </row>
-    <row r="69" spans="1:12">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
         <v>5</v>
       </c>
@@ -2627,7 +2629,7 @@
       <c r="K69" s="5"/>
       <c r="L69" s="5"/>
     </row>
-    <row r="70" spans="1:12">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70" s="11" t="s">
         <v>0</v>
       </c>
@@ -2652,7 +2654,7 @@
       <c r="K70" s="5"/>
       <c r="L70" s="5"/>
     </row>
-    <row r="71" spans="1:12">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71" s="11"/>
       <c r="B71" s="5"/>
       <c r="C71" s="5"/>
@@ -2669,7 +2671,7 @@
       <c r="K71" s="5"/>
       <c r="L71" s="5"/>
     </row>
-    <row r="72" spans="1:12">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72" s="11"/>
       <c r="B72" s="5"/>
       <c r="C72" s="5"/>
@@ -2686,7 +2688,7 @@
       <c r="K72" s="5"/>
       <c r="L72" s="5"/>
     </row>
-    <row r="73" spans="1:12">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73" s="9" t="s">
         <v>76</v>
       </c>
@@ -2705,7 +2707,7 @@
       <c r="K73" s="5"/>
       <c r="L73" s="5"/>
     </row>
-    <row r="74" spans="1:12">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
         <v>77</v>
       </c>
@@ -2726,7 +2728,7 @@
       <c r="K74" s="5"/>
       <c r="L74" s="5"/>
     </row>
-    <row r="75" spans="1:12">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
         <v>79</v>
       </c>
@@ -2747,7 +2749,7 @@
       <c r="K75" s="5"/>
       <c r="L75" s="5"/>
     </row>
-    <row r="76" spans="1:12">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
         <v>78</v>
       </c>
@@ -2768,7 +2770,7 @@
       <c r="K76" s="5"/>
       <c r="L76" s="5"/>
     </row>
-    <row r="77" spans="1:12">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77" s="11" t="s">
         <v>74</v>
       </c>
@@ -2789,7 +2791,7 @@
       <c r="K77" s="5"/>
       <c r="L77" s="5"/>
     </row>
-    <row r="78" spans="1:12">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
         <v>73</v>
       </c>
@@ -2810,7 +2812,7 @@
       <c r="K78" s="5"/>
       <c r="L78" s="5"/>
     </row>
-    <row r="79" spans="1:12">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
         <v>75</v>
       </c>
@@ -2831,7 +2833,7 @@
       <c r="K79" s="5"/>
       <c r="L79" s="5"/>
     </row>
-    <row r="80" spans="1:12">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="1"/>
       <c r="C80" s="1"/>
@@ -2848,7 +2850,7 @@
       <c r="K80" s="5"/>
       <c r="L80" s="5"/>
     </row>
-    <row r="81" spans="1:12">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="1"/>
       <c r="C81" s="1"/>
@@ -2865,7 +2867,7 @@
       <c r="K81" s="5"/>
       <c r="L81" s="5"/>
     </row>
-    <row r="82" spans="1:12">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82" s="9" t="s">
         <v>32</v>
       </c>
@@ -2889,7 +2891,7 @@
       <c r="K82" s="6"/>
       <c r="L82" s="5"/>
     </row>
-    <row r="83" spans="1:12">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
         <v>18</v>
       </c>
@@ -2911,7 +2913,7 @@
       <c r="K83" s="6"/>
       <c r="L83" s="5"/>
     </row>
-    <row r="84" spans="1:12">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
         <v>29</v>
       </c>
@@ -2933,7 +2935,7 @@
       <c r="K84" s="6"/>
       <c r="L84" s="5"/>
     </row>
-    <row r="85" spans="1:12">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85" s="11"/>
       <c r="B85" s="5"/>
       <c r="C85" s="5"/>
@@ -2947,7 +2949,7 @@
       <c r="K85" s="6"/>
       <c r="L85" s="5"/>
     </row>
-    <row r="86" spans="1:12">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86" s="11"/>
       <c r="B86" s="5"/>
       <c r="C86" s="5"/>
@@ -2961,80 +2963,80 @@
       <c r="K86" s="5"/>
       <c r="L86" s="5"/>
     </row>
-    <row r="87" spans="1:12">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87" s="14" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88" s="12" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89" s="12"/>
     </row>
-    <row r="90" spans="1:12">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
     </row>
-    <row r="91" spans="1:12">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91" s="12"/>
     </row>
-    <row r="92" spans="1:12">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92" s="12"/>
     </row>
-    <row r="93" spans="1:12">
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93" s="12"/>
     </row>
-    <row r="94" spans="1:12">
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94" s="12"/>
     </row>
-    <row r="95" spans="1:12">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95" s="12"/>
     </row>
-    <row r="96" spans="1:12">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96" s="12"/>
     </row>
-    <row r="97" spans="1:1">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="12"/>
     </row>
-    <row r="98" spans="1:1">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="12"/>
     </row>
-    <row r="99" spans="1:1">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="12"/>
     </row>
-    <row r="100" spans="1:1">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="12"/>
     </row>
-    <row r="101" spans="1:1">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="12"/>
     </row>
-    <row r="102" spans="1:1">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="12"/>
     </row>
-    <row r="103" spans="1:1">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="12"/>
     </row>
-    <row r="104" spans="1:1">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="12"/>
     </row>
-    <row r="105" spans="1:1">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="12"/>
     </row>
-    <row r="106" spans="1:1">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="12"/>
     </row>
-    <row r="107" spans="1:1">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="12"/>
     </row>
-    <row r="108" spans="1:1">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="12"/>
     </row>
-    <row r="109" spans="1:1">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="12"/>
     </row>
-    <row r="110" spans="1:1">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="13"/>
     </row>
   </sheetData>
@@ -3059,7 +3061,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L6 K4 H6:J6">
+  <conditionalFormatting sqref="K4 L6 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>
@@ -3130,7 +3132,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>
@@ -3147,7 +3149,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Camera x/z translation. Plus WIP
WIP for refactoring code blocks.
</commit_message>
<xml_diff>
--- a/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
+++ b/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="4545" yWindow="1575" windowWidth="30375" windowHeight="17280"/>
+    <workbookView xWindow="6405" yWindow="1575" windowWidth="30375" windowHeight="17280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="98">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>III</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Getting and handling Input Information via Message Queue. (Custom toggling included). (Win32 Project) </t>
   </si>
 </sst>
 </file>
@@ -671,7 +677,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -723,7 +729,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -952,7 +958,7 @@
   <dimension ref="A1:L110"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="E62" sqref="E62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1093,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1095,7 +1101,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>24</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1232,7 +1238,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1513,7 +1519,7 @@
         <v>3</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F20" s="3"/>
       <c r="G20" s="16">
@@ -2339,7 +2345,9 @@
       <c r="L56" s="5"/>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A57" s="8"/>
+      <c r="A57" s="8" t="s">
+        <v>97</v>
+      </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
       <c r="D57" s="1"/>
@@ -2405,12 +2413,14 @@
         <v>1</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="F60" s="3"/>
+        <v>96</v>
+      </c>
+      <c r="F60" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G60" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H60" s="5"/>
       <c r="I60" s="5"/>
@@ -2432,7 +2442,7 @@
         <v>1</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F61" s="3"/>
       <c r="G61" s="16">
@@ -2484,7 +2494,7 @@
         <v>1</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="F63" s="3"/>
       <c r="G63" s="16">
@@ -2904,7 +2914,9 @@
       <c r="D83" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E83" s="3"/>
+      <c r="E83" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
@@ -2926,7 +2938,9 @@
       <c r="D84" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E84" s="3"/>
+      <c r="E84" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>

</xml_diff>

<commit_message>
Press 'T' to track. (hardcoded to default 'cubeworld')
</commit_message>
<xml_diff>
--- a/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
+++ b/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E62" sqref="E62"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -2350,12 +2350,18 @@
       </c>
       <c r="B57" s="1"/>
       <c r="C57" s="1"/>
-      <c r="D57" s="1"/>
-      <c r="E57" s="2"/>
-      <c r="F57" s="3"/>
+      <c r="D57" s="1">
+        <v>1</v>
+      </c>
+      <c r="E57" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F57" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G57" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H57" s="5"/>
       <c r="I57" s="5"/>
@@ -2444,10 +2450,12 @@
       <c r="E61" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F61" s="3"/>
+      <c r="F61" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G61" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61" s="5"/>
       <c r="I61" s="5"/>
@@ -2496,10 +2504,12 @@
       <c r="E63" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="F63" s="3"/>
+      <c r="F63" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G63" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H63" s="5"/>
       <c r="I63" s="5"/>

</xml_diff>

<commit_message>
Added model loading. CLosing up
</commit_message>
<xml_diff>
--- a/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
+++ b/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="6405" yWindow="1575" windowWidth="30375" windowHeight="17280"/>
+    <workbookView xWindow="7335" yWindow="1575" windowWidth="30375" windowHeight="17280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="98">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -957,8 +957,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="E55" sqref="E55"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1238,7 +1238,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1518,9 +1518,7 @@
       <c r="D20" s="5">
         <v>3</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>96</v>
-      </c>
+      <c r="E20" s="2"/>
       <c r="F20" s="3"/>
       <c r="G20" s="16">
         <f t="shared" si="0"/>
@@ -2307,11 +2305,15 @@
       <c r="D55" s="5">
         <v>3</v>
       </c>
-      <c r="E55" s="2"/>
-      <c r="F55" s="3"/>
+      <c r="E55" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F55" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G55" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="H55" s="5"/>
       <c r="I55" s="5"/>
@@ -2332,11 +2334,15 @@
       <c r="D56" s="5">
         <v>4</v>
       </c>
-      <c r="E56" s="2"/>
-      <c r="F56" s="3"/>
+      <c r="E56" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F56" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G56" s="16">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="H56" s="5"/>
       <c r="I56" s="5"/>
@@ -2948,9 +2954,7 @@
       <c r="D84" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E84" s="3" t="s">
-        <v>90</v>
-      </c>
+      <c r="E84" s="3"/>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
@@ -3085,7 +3089,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
GS_Shader for Multi Viewport and instancing (WIP)
</commit_message>
<xml_diff>
--- a/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
+++ b/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="10125" yWindow="1575" windowWidth="30375" windowHeight="17280"/>
+    <workbookView xWindow="11055" yWindow="1575" windowWidth="30375" windowHeight="17280"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -951,8 +951,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3083,7 +3083,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4 L6 H6:J6">
+  <conditionalFormatting sqref="L6 K4 H6:J6">
     <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
Multi-Viewport rendering form GS
</commit_message>
<xml_diff>
--- a/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
+++ b/RiveraBrenesYaniel_Dev_IV_Project_Rubric.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18229"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="18326"/>
   <workbookPr filterPrivacy="1" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="11985" yWindow="1575" windowWidth="30375" windowHeight="17280"/>
+    <workbookView xWindow="13845" yWindow="1575" windowWidth="30375" windowHeight="17280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -21,12 +21,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0" shapeId="0">
+    <comment ref="A1" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -41,7 +41,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A2" authorId="0" shapeId="0">
+    <comment ref="A2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A66" authorId="0" shapeId="0">
+    <comment ref="A66" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="99">
   <si>
     <t>Apply a post process routine via pixel shader (eg Blur or Custom Pixel Maipulations)</t>
   </si>
@@ -375,12 +375,18 @@
   </si>
   <si>
     <t>II</t>
+  </si>
+  <si>
+    <t>https://www.braynzarsoft.net/viewtutorial/q16390-simple-lighting</t>
+  </si>
+  <si>
+    <t>III</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -951,11 +957,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E64" sqref="E64"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1090,7 +1096,7 @@
       </c>
       <c r="J4" s="17">
         <f>IF(SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84) &gt; 18, 18, SUMIF(E4:E81,"=III",G4:G81) + SUMIF(E83:E84, "X",B83:B84))</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="K4" s="17">
         <f>SUM(H6,I6,J6)</f>
@@ -1098,7 +1104,7 @@
       </c>
       <c r="L4" s="17">
         <f>SUM(G4:G81) + SUMIF(C83:C84, "X",B83:B84) + SUMIF(D83:D84, "X",B83:B84) + SUMIF(E83:E84, "X",B83:B84)</f>
-        <v>40</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -1235,7 +1241,7 @@
       </c>
       <c r="J8" s="17">
         <f>J4+IF(J4 &lt; 18, IF(I10+J4 &gt; 18, 18- J4, I10),0)</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="5"/>
@@ -1284,11 +1290,15 @@
       <c r="D10" s="5">
         <v>1</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3"/>
+      <c r="E10" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="G10" s="16">
         <f xml:space="preserve"> IF(EXACT(F10,"X"),IF(EXACT(E10,"I"),$B10,IF(EXACT(E10,"II"),$C10,IF(EXACT(E10,"III"),$D10,0))),0)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" s="19">
         <f>IF(K4+H4 - 18 &gt; 0, K4+H4 - 18, 0)</f>
@@ -1622,9 +1632,7 @@
       <c r="D25" s="5">
         <v>2</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>94</v>
-      </c>
+      <c r="E25" s="2"/>
       <c r="F25" s="3"/>
       <c r="G25" s="16">
         <f t="shared" si="0"/>
@@ -2933,7 +2941,9 @@
       <c r="D83" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E83" s="3"/>
+      <c r="E83" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="F83" s="5"/>
       <c r="G83" s="5"/>
       <c r="H83" s="5"/>
@@ -2955,7 +2965,9 @@
       <c r="D84" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="E84" s="3"/>
+      <c r="E84" s="3" t="s">
+        <v>90</v>
+      </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
@@ -3003,7 +3015,9 @@
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A89" s="12"/>
+      <c r="A89" s="12" t="s">
+        <v>97</v>
+      </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90" s="12"/>
@@ -3129,18 +3143,18 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="4">
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C83:E84 F4:F81">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with capital X!" sqref="C83:E84 F4:F81" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>IF(EXACT(C4,"X"),TRUE,FALSE)</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D80:D81 D3:D78 B3:C81">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D80:D81 D3:D78 B3:C81" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>1</formula1>
       <formula2>5</formula2>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D79">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Out of Range" error="Points for any one custom feature_x000a_may only range from 1 - 5." sqref="D79" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>1</formula1>
       <formula2>6</formula2>
     </dataValidation>
-    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E81">
+    <dataValidation type="custom" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid" error="Can only be marked with roman numerals I, II, or III!" sqref="E4:E81" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>IF(EXACT(E4,"I"),TRUE,IF(EXACT(E4,"II"),TRUE,IF(EXACT(E4,"III"),TRUE,FALSE)))</formula1>
     </dataValidation>
   </dataValidations>
@@ -3156,7 +3170,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -3173,7 +3187,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>